<commit_message>
update activity log, visitor, pengumuman, testimonial
</commit_message>
<xml_diff>
--- a/public/Data Guru/teacher.xlsx
+++ b/public/Data Guru/teacher.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DF5373-EAA7-4FAE-A334-148277FECEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Guru" sheetId="1" r:id="rId4"/>
+    <sheet name="Data Guru" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>No</t>
   </si>
@@ -41,152 +57,150 @@
     <t>Mata Pelajaran</t>
   </si>
   <si>
-    <t>Kira Pollich Sr.</t>
-  </si>
-  <si>
-    <t>830.618.3708</t>
-  </si>
-  <si>
-    <t>1655 Donnie Spurs Suite 258 Aliceside, NV 53078-0428</t>
-  </si>
-  <si>
-    <t>23/10/2006</t>
+    <t>Ms. Juanita Nicolas</t>
+  </si>
+  <si>
+    <t>(434) 833-4871</t>
+  </si>
+  <si>
+    <t>8429 Vidal Pass Apt. 251 Matteoberg, NE 77857-7294</t>
+  </si>
+  <si>
+    <t>31/12/2012</t>
   </si>
   <si>
     <t>Laki-laki</t>
   </si>
   <si>
+    <t>IPS</t>
+  </si>
+  <si>
+    <t>Brooke Cartwright</t>
+  </si>
+  <si>
+    <t>484.650.5253</t>
+  </si>
+  <si>
+    <t>7525 Kirk Crest Apt. 883 Herzoghaven, AR 54122</t>
+  </si>
+  <si>
+    <t>22/09/1993</t>
+  </si>
+  <si>
+    <t>Matematika</t>
+  </si>
+  <si>
+    <t>Mr. Jimmy Cassin</t>
+  </si>
+  <si>
+    <t>743-622-8553</t>
+  </si>
+  <si>
+    <t>625 Schamberger Expressway Murazikmouth, CO 49556-3593</t>
+  </si>
+  <si>
+    <t>28/02/1980</t>
+  </si>
+  <si>
+    <t>Miss Patricia Wisoky</t>
+  </si>
+  <si>
+    <t>+1.224.464.6790</t>
+  </si>
+  <si>
+    <t>6807 Gretchen Plain Apt. 845 Maudemouth, AZ 79375-9082</t>
+  </si>
+  <si>
+    <t>15/06/2003</t>
+  </si>
+  <si>
+    <t>Doyle Kozey</t>
+  </si>
+  <si>
+    <t>1-573-444-7287</t>
+  </si>
+  <si>
+    <t>66455 Hartmann Junction Apt. 272 Reeseton, NC 35517-8518</t>
+  </si>
+  <si>
+    <t>04/06/1970</t>
+  </si>
+  <si>
+    <t>Adrian Zemlak Sr.</t>
+  </si>
+  <si>
+    <t>848-378-8645</t>
+  </si>
+  <si>
+    <t>510 Swift Glens Apt. 949 Muellerstad, IN 06429</t>
+  </si>
+  <si>
+    <t>28/05/1972</t>
+  </si>
+  <si>
+    <t>Perempuan</t>
+  </si>
+  <si>
     <t>IPA</t>
   </si>
   <si>
-    <t>Daren Frami I</t>
-  </si>
-  <si>
-    <t>425-744-2468</t>
-  </si>
-  <si>
-    <t>53333 Jeanie Stream Nilshaven, MN 89648</t>
-  </si>
-  <si>
-    <t>25/07/2012</t>
-  </si>
-  <si>
-    <t>Perempuan</t>
+    <t>Miss Helen Wehner I</t>
+  </si>
+  <si>
+    <t>361-555-7396</t>
+  </si>
+  <si>
+    <t>7627 Thomas Manors Suite 276 Port Floyberg, NV 56744</t>
+  </si>
+  <si>
+    <t>03/02/2009</t>
   </si>
   <si>
     <t>Bahasa Inggris</t>
   </si>
   <si>
-    <t>Ms. Tabitha Cole</t>
-  </si>
-  <si>
-    <t>1-321-390-8635</t>
-  </si>
-  <si>
-    <t>4532 Kovacek Mills Jeffshire, HI 61518</t>
-  </si>
-  <si>
-    <t>13/08/1980</t>
-  </si>
-  <si>
-    <t>Matematika</t>
-  </si>
-  <si>
-    <t>Jailyn McDermott</t>
-  </si>
-  <si>
-    <t>762-551-7408</t>
-  </si>
-  <si>
-    <t>65678 Yost Square South Royville, TX 06296-2350</t>
-  </si>
-  <si>
-    <t>22/05/1971</t>
-  </si>
-  <si>
-    <t>Sebastian Dicki</t>
-  </si>
-  <si>
-    <t>458-431-8191</t>
-  </si>
-  <si>
-    <t>317 Gaylord Inlet Lake Izaiah, WI 27090-2245</t>
-  </si>
-  <si>
-    <t>17/04/2017</t>
-  </si>
-  <si>
-    <t>IPS</t>
-  </si>
-  <si>
-    <t>Eli Ferry</t>
-  </si>
-  <si>
-    <t>23286 Leannon Mount Corkerybury, NV 56184</t>
-  </si>
-  <si>
-    <t>22/07/1987</t>
-  </si>
-  <si>
-    <t>Freeda Schuster IV</t>
-  </si>
-  <si>
-    <t>+1 (364) 752-6731</t>
-  </si>
-  <si>
-    <t>332 Stracke Crossing New Ressiebury, NY 80909-3618</t>
-  </si>
-  <si>
-    <t>05/05/1987</t>
-  </si>
-  <si>
-    <t>Clay Rohan</t>
-  </si>
-  <si>
-    <t>+1-445-543-3036</t>
-  </si>
-  <si>
-    <t>5091 Kuhn Underpass Gladysside, RI 87417</t>
-  </si>
-  <si>
-    <t>04/09/1976</t>
-  </si>
-  <si>
-    <t>Tyshawn Littel</t>
-  </si>
-  <si>
-    <t>678.980.2900</t>
-  </si>
-  <si>
-    <t>86894 Bernhard Club Apt. 629 Strosinchester, FL 09824</t>
-  </si>
-  <si>
-    <t>04/08/2017</t>
-  </si>
-  <si>
-    <t>Prof. Lenna Volkman</t>
-  </si>
-  <si>
-    <t>+1-351-439-5644</t>
-  </si>
-  <si>
-    <t>284 Grimes Forge Suite 280 New Oma, NM 90952</t>
-  </si>
-  <si>
-    <t>26/04/1983</t>
+    <t>Dr. Anita Jacobson II</t>
+  </si>
+  <si>
+    <t>1-219-951-5801</t>
+  </si>
+  <si>
+    <t>816 Fredrick Haven Apt. 569 North Magnolia, MI 45288</t>
+  </si>
+  <si>
+    <t>03/06/2008</t>
+  </si>
+  <si>
+    <t>Prof. Meghan Nitzsche</t>
+  </si>
+  <si>
+    <t>484-952-0406</t>
+  </si>
+  <si>
+    <t>763 Vernon Well Nadermouth, IA 37870</t>
+  </si>
+  <si>
+    <t>23/04/2022</t>
+  </si>
+  <si>
+    <t>Elaina Schneider II</t>
+  </si>
+  <si>
+    <t>+1 (223) 951-4941</t>
+  </si>
+  <si>
+    <t>573 Christy Locks Suite 224 West Opal, WV 64740</t>
+  </si>
+  <si>
+    <t>29/11/1987</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -213,13 +227,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -509,29 +531,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="23.423" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="21.138" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="63.556" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="16.425" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -557,12 +575,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>12649954544</v>
+        <v>3408086123</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -583,12 +601,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>43085856529</v>
+        <v>6151987329</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -603,122 +621,122 @@
         <v>17</v>
       </c>
       <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>27709815777</v>
+        <v>9804246183</v>
       </c>
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>85711752246</v>
+        <v>5265193590</v>
       </c>
       <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
       <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
         <v>18</v>
       </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>75250442714</v>
+        <v>6989471824</v>
       </c>
       <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>44318626158</v>
+        <v>4884862803</v>
       </c>
       <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="D7">
-        <v>15742994659</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>35</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>36</v>
       </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>83691800021</v>
+        <v>8177716152</v>
       </c>
       <c r="C8" t="s">
         <v>37</v>
@@ -733,102 +751,91 @@
         <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>90323182668</v>
+        <v>1588414299</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>50487633830</v>
+        <v>8118838146</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>69104197045</v>
+        <v>6824091044</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
         <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
message & update student
</commit_message>
<xml_diff>
--- a/public/Data Guru/teacher.xlsx
+++ b/public/Data Guru/teacher.xlsx
@@ -1,37 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DF5373-EAA7-4FAE-A334-148277FECEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Guru" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Guru" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" forceFullCalc="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>No</t>
   </si>
@@ -57,150 +41,152 @@
     <t>Mata Pelajaran</t>
   </si>
   <si>
-    <t>Ms. Juanita Nicolas</t>
-  </si>
-  <si>
-    <t>(434) 833-4871</t>
-  </si>
-  <si>
-    <t>8429 Vidal Pass Apt. 251 Matteoberg, NE 77857-7294</t>
-  </si>
-  <si>
-    <t>31/12/2012</t>
+    <t>Kira Pollich Sr.</t>
+  </si>
+  <si>
+    <t>830.618.3708</t>
+  </si>
+  <si>
+    <t>1655 Donnie Spurs Suite 258 Aliceside, NV 53078-0428</t>
+  </si>
+  <si>
+    <t>23/10/2006</t>
   </si>
   <si>
     <t>Laki-laki</t>
   </si>
   <si>
+    <t>IPA</t>
+  </si>
+  <si>
+    <t>Daren Frami I</t>
+  </si>
+  <si>
+    <t>425-744-2468</t>
+  </si>
+  <si>
+    <t>53333 Jeanie Stream Nilshaven, MN 89648</t>
+  </si>
+  <si>
+    <t>25/07/2012</t>
+  </si>
+  <si>
+    <t>Perempuan</t>
+  </si>
+  <si>
+    <t>Bahasa Inggris</t>
+  </si>
+  <si>
+    <t>Ms. Tabitha Cole</t>
+  </si>
+  <si>
+    <t>1-321-390-8635</t>
+  </si>
+  <si>
+    <t>4532 Kovacek Mills Jeffshire, HI 61518</t>
+  </si>
+  <si>
+    <t>13/08/1980</t>
+  </si>
+  <si>
+    <t>Matematika</t>
+  </si>
+  <si>
+    <t>Jailyn McDermott</t>
+  </si>
+  <si>
+    <t>762-551-7408</t>
+  </si>
+  <si>
+    <t>65678 Yost Square South Royville, TX 06296-2350</t>
+  </si>
+  <si>
+    <t>22/05/1971</t>
+  </si>
+  <si>
+    <t>Sebastian Dicki</t>
+  </si>
+  <si>
+    <t>458-431-8191</t>
+  </si>
+  <si>
+    <t>317 Gaylord Inlet Lake Izaiah, WI 27090-2245</t>
+  </si>
+  <si>
+    <t>17/04/2017</t>
+  </si>
+  <si>
     <t>IPS</t>
   </si>
   <si>
-    <t>Brooke Cartwright</t>
-  </si>
-  <si>
-    <t>484.650.5253</t>
-  </si>
-  <si>
-    <t>7525 Kirk Crest Apt. 883 Herzoghaven, AR 54122</t>
-  </si>
-  <si>
-    <t>22/09/1993</t>
-  </si>
-  <si>
-    <t>Matematika</t>
-  </si>
-  <si>
-    <t>Mr. Jimmy Cassin</t>
-  </si>
-  <si>
-    <t>743-622-8553</t>
-  </si>
-  <si>
-    <t>625 Schamberger Expressway Murazikmouth, CO 49556-3593</t>
-  </si>
-  <si>
-    <t>28/02/1980</t>
-  </si>
-  <si>
-    <t>Miss Patricia Wisoky</t>
-  </si>
-  <si>
-    <t>+1.224.464.6790</t>
-  </si>
-  <si>
-    <t>6807 Gretchen Plain Apt. 845 Maudemouth, AZ 79375-9082</t>
-  </si>
-  <si>
-    <t>15/06/2003</t>
-  </si>
-  <si>
-    <t>Doyle Kozey</t>
-  </si>
-  <si>
-    <t>1-573-444-7287</t>
-  </si>
-  <si>
-    <t>66455 Hartmann Junction Apt. 272 Reeseton, NC 35517-8518</t>
-  </si>
-  <si>
-    <t>04/06/1970</t>
-  </si>
-  <si>
-    <t>Adrian Zemlak Sr.</t>
-  </si>
-  <si>
-    <t>848-378-8645</t>
-  </si>
-  <si>
-    <t>510 Swift Glens Apt. 949 Muellerstad, IN 06429</t>
-  </si>
-  <si>
-    <t>28/05/1972</t>
-  </si>
-  <si>
-    <t>Perempuan</t>
-  </si>
-  <si>
-    <t>IPA</t>
-  </si>
-  <si>
-    <t>Miss Helen Wehner I</t>
-  </si>
-  <si>
-    <t>361-555-7396</t>
-  </si>
-  <si>
-    <t>7627 Thomas Manors Suite 276 Port Floyberg, NV 56744</t>
-  </si>
-  <si>
-    <t>03/02/2009</t>
-  </si>
-  <si>
-    <t>Bahasa Inggris</t>
-  </si>
-  <si>
-    <t>Dr. Anita Jacobson II</t>
-  </si>
-  <si>
-    <t>1-219-951-5801</t>
-  </si>
-  <si>
-    <t>816 Fredrick Haven Apt. 569 North Magnolia, MI 45288</t>
-  </si>
-  <si>
-    <t>03/06/2008</t>
-  </si>
-  <si>
-    <t>Prof. Meghan Nitzsche</t>
-  </si>
-  <si>
-    <t>484-952-0406</t>
-  </si>
-  <si>
-    <t>763 Vernon Well Nadermouth, IA 37870</t>
-  </si>
-  <si>
-    <t>23/04/2022</t>
-  </si>
-  <si>
-    <t>Elaina Schneider II</t>
-  </si>
-  <si>
-    <t>+1 (223) 951-4941</t>
-  </si>
-  <si>
-    <t>573 Christy Locks Suite 224 West Opal, WV 64740</t>
-  </si>
-  <si>
-    <t>29/11/1987</t>
+    <t>Eli Ferry</t>
+  </si>
+  <si>
+    <t>23286 Leannon Mount Corkerybury, NV 56184</t>
+  </si>
+  <si>
+    <t>22/07/1987</t>
+  </si>
+  <si>
+    <t>Freeda Schuster IV</t>
+  </si>
+  <si>
+    <t>+1 (364) 752-6731</t>
+  </si>
+  <si>
+    <t>332 Stracke Crossing New Ressiebury, NY 80909-3618</t>
+  </si>
+  <si>
+    <t>05/05/1987</t>
+  </si>
+  <si>
+    <t>Clay Rohan</t>
+  </si>
+  <si>
+    <t>+1-445-543-3036</t>
+  </si>
+  <si>
+    <t>5091 Kuhn Underpass Gladysside, RI 87417</t>
+  </si>
+  <si>
+    <t>04/09/1976</t>
+  </si>
+  <si>
+    <t>Tyshawn Littel</t>
+  </si>
+  <si>
+    <t>678.980.2900</t>
+  </si>
+  <si>
+    <t>86894 Bernhard Club Apt. 629 Strosinchester, FL 09824</t>
+  </si>
+  <si>
+    <t>04/08/2017</t>
+  </si>
+  <si>
+    <t>Prof. Lenna Volkman</t>
+  </si>
+  <si>
+    <t>+1-351-439-5644</t>
+  </si>
+  <si>
+    <t>284 Grimes Forge Suite 280 New Oma, NM 90952</t>
+  </si>
+  <si>
+    <t>26/04/1983</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -227,21 +213,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -531,25 +509,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="63.556" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="17.567" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,12 +557,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>3408086123</v>
+        <v>12649954544</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -601,12 +583,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>6151987329</v>
+        <v>43085856529</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -621,122 +603,122 @@
         <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>9804246183</v>
+        <v>27709815777</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>5265193590</v>
+        <v>85711752246</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>6989471824</v>
+        <v>75250442714</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>4884862803</v>
+        <v>44318626158</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>15742994659</v>
       </c>
       <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
         <v>33</v>
       </c>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8">
-        <v>8177716152</v>
+        <v>83691800021</v>
       </c>
       <c r="C8" t="s">
         <v>37</v>
@@ -751,91 +733,102 @@
         <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>1588414299</v>
+        <v>90323182668</v>
       </c>
       <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>43</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>44</v>
       </c>
-      <c r="F9" t="s">
-        <v>45</v>
-      </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10">
-        <v>8118838146</v>
+        <v>50487633830</v>
       </c>
       <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
         <v>46</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>47</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>48</v>
       </c>
-      <c r="F10" t="s">
-        <v>49</v>
-      </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>11</v>
       </c>
       <c r="B11">
-        <v>6824091044</v>
+        <v>69104197045</v>
       </c>
       <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>51</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>52</v>
-      </c>
-      <c r="F11" t="s">
-        <v>53</v>
       </c>
       <c r="G11" t="s">
         <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>